<commit_message>
reduced trials from 100 to 50
</commit_message>
<xml_diff>
--- a/html/resources/mentalrotationstimuli.xlsx
+++ b/html/resources/mentalrotationstimuli.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/files/experiments/mentalrotationfinal/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28C07BAD-A73F-A74E-B016-AE981E69330A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="800" windowWidth="28140" windowHeight="19680" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="28140" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>imagefile</t>
   </si>
@@ -184,162 +190,12 @@
   </si>
   <si>
     <t>i23_50.jpg</t>
-  </si>
-  <si>
-    <t>i23_150_R.jpg</t>
-  </si>
-  <si>
-    <t>i24_50.jpg</t>
-  </si>
-  <si>
-    <t>i24_150_R.jpg</t>
-  </si>
-  <si>
-    <t>i25_0.jpg</t>
-  </si>
-  <si>
-    <t>i25_50.jpg</t>
-  </si>
-  <si>
-    <t>i25_150_R.jpg</t>
-  </si>
-  <si>
-    <t>i26_50.jpg</t>
-  </si>
-  <si>
-    <t>i26_150_R.jpg</t>
-  </si>
-  <si>
-    <t>i27_50.jpg</t>
-  </si>
-  <si>
-    <t>i27_150_R.jpg</t>
-  </si>
-  <si>
-    <t>i28_50.jpg</t>
-  </si>
-  <si>
-    <t>i28_150.jpg</t>
-  </si>
-  <si>
-    <t>i29_0.jpg</t>
-  </si>
-  <si>
-    <t>i29_50.jpg</t>
-  </si>
-  <si>
-    <t>i29_150.jpg</t>
-  </si>
-  <si>
-    <t>i30_50.jpg</t>
-  </si>
-  <si>
-    <t>i30_150.jpg</t>
-  </si>
-  <si>
-    <t>i31_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i31_150.jpg</t>
-  </si>
-  <si>
-    <t>i32_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i32_150.jpg</t>
-  </si>
-  <si>
-    <t>i33_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i33_150.jpg</t>
-  </si>
-  <si>
-    <t>i34_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i34_150.jpg</t>
-  </si>
-  <si>
-    <t>i35_0.jpg</t>
-  </si>
-  <si>
-    <t>i35_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i35_150.jpg</t>
-  </si>
-  <si>
-    <t>i36_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i36_150.jpg</t>
-  </si>
-  <si>
-    <t>i37_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i37_150.jpg</t>
-  </si>
-  <si>
-    <t>i38_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i38_150.jpg</t>
-  </si>
-  <si>
-    <t>i39_0.jpg</t>
-  </si>
-  <si>
-    <t>i39_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i39_150.jpg</t>
-  </si>
-  <si>
-    <t>i40_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i40_150.jpg</t>
-  </si>
-  <si>
-    <t>i41_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i41_150.jpg</t>
-  </si>
-  <si>
-    <t>i42_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i42_150.jpg</t>
-  </si>
-  <si>
-    <t>i43_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i44_0.jpg</t>
-  </si>
-  <si>
-    <t>i44_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i45_100_R.jpg</t>
-  </si>
-  <si>
-    <t>i46_100.jpg</t>
-  </si>
-  <si>
-    <t>i47_100.jpg</t>
-  </si>
-  <si>
-    <t>i48_100.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -388,6 +244,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -712,19 +576,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -746,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -757,7 +621,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -768,7 +632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -779,7 +643,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -790,7 +654,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -801,7 +665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -812,7 +676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -823,7 +687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -834,7 +698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -845,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -856,7 +720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -867,7 +731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -878,7 +742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -889,7 +753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -900,7 +764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -911,7 +775,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -922,7 +786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -933,7 +797,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -944,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -955,7 +819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -966,7 +830,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -977,7 +841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -988,7 +852,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -999,7 +863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1010,7 +874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1021,7 +885,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1032,7 +896,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1043,7 +907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1054,7 +918,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1065,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1076,7 +940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1087,7 +951,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1098,7 +962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1109,7 +973,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1120,7 +984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +995,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1142,7 +1006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1153,7 +1017,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1164,7 +1028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1175,7 +1039,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1186,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1197,7 +1061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1208,7 +1072,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1219,7 +1083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1230,7 +1094,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1241,7 +1105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1252,7 +1116,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1263,7 +1127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1274,7 +1138,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1283,556 +1147,6 @@
       </c>
       <c r="C51">
         <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>78</v>
-      </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>82</v>
-      </c>
-      <c r="B79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>89</v>
-      </c>
-      <c r="B86" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>90</v>
-      </c>
-      <c r="B87" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>91</v>
-      </c>
-      <c r="B88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>92</v>
-      </c>
-      <c r="B89" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>93</v>
-      </c>
-      <c r="B90" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>94</v>
-      </c>
-      <c r="B91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>95</v>
-      </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>97</v>
-      </c>
-      <c r="B94" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>99</v>
-      </c>
-      <c r="B96" t="s">
-        <v>3</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>100</v>
-      </c>
-      <c r="B97" t="s">
-        <v>4</v>
-      </c>
-      <c r="C97">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>101</v>
-      </c>
-      <c r="B98" t="s">
-        <v>4</v>
-      </c>
-      <c r="C98">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>102</v>
-      </c>
-      <c r="B99" t="s">
-        <v>3</v>
-      </c>
-      <c r="C99">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>103</v>
-      </c>
-      <c r="B100" t="s">
-        <v>3</v>
-      </c>
-      <c r="C100">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>